<commit_message>
Bulk Deposit - New Narration
</commit_message>
<xml_diff>
--- a/mfi/bulkWork/files/bulk_deposit.xlsx
+++ b/mfi/bulkWork/files/bulk_deposit.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Severs\Xamp\htdocs\sekani\mfi\bulkWork\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sekani\mfi\bulkWork\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11EF384-0522-484F-82D1-C47147593757}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D697355F-BEA3-4F7F-BC0E-7B8E39E9B67F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,9 +35,6 @@
     <t>Account Number</t>
   </si>
   <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -52,12 +48,15 @@
   </si>
   <si>
     <t>Transaction Type</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -411,11 +410,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCBAD71-3F5A-49A5-9049-40BF44FAE0F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,22 +441,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>